<commit_message>
scraper.py now fully functional
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rami/Desktop/fall 2022/DATABASE SYSTEMS/basketball_DB_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7AF9E-A18F-FB45-B3B7-65BD6BD40744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F099058E-0319-2848-A234-666C9CD2D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{D941CE5F-CAE8-544D-853E-19BD962595B2}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{D941CE5F-CAE8-544D-853E-19BD962595B2}"/>
   </bookViews>
   <sheets>
     <sheet name="season" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47503F77-37C2-BA46-B635-358856187CBC}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1997</v>
+        <v>1966</v>
       </c>
       <c r="B2">
         <v>66</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1998</v>
+        <v>1967</v>
       </c>
       <c r="B3">
         <v>67</v>
@@ -483,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D97BCB7-5735-D14B-AD1E-0348172DFE9B}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>